<commit_message>
modificação na formulação do problema e conferencia das equações. Problema nao convergiu
</commit_message>
<xml_diff>
--- a/DATA/teste.xlsx
+++ b/DATA/teste.xlsx
@@ -378,7 +378,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -441,7 +441,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>-40000</v>
+        <v>40000</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>14</v>

</xml_diff>